<commit_message>
Updates test reports and test files.
</commit_message>
<xml_diff>
--- a/tests/tests_manual/AssetDsinExcel1.xlsx
+++ b/tests/tests_manual/AssetDsinExcel1.xlsx
@@ -1,42 +1,114 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr codeName="ThisWorkbook"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\RSA\draw\tests\tests_manual\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{EF362D70-DE43-438A-9433-5C20520C31FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="-23832" yWindow="-2112" windowWidth="21600" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
     <sheet name="Dependency" sheetId="1" r:id="rId1"/>
     <sheet name="Parameters" sheetId="2" r:id="rId2"/>
   </sheets>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
-<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
-  <metadataTypes count="1">
-    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
-  </metadataTypes>
-  <futureMetadata name="XLDAPR" count="1">
-    <bk>
-      <extLst>
-        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
-          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
-        </ext>
-      </extLst>
-    </bk>
-  </futureMetadata>
-  <cellMetadata count="1">
-    <bk>
-      <rc t="1" v="0"/>
-    </bk>
-  </cellMetadata>
-</metadata>
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="27">
+  <si>
+    <t>AssetList</t>
+  </si>
+  <si>
+    <t>AssetType</t>
+  </si>
+  <si>
+    <t>AssetComment</t>
+  </si>
+  <si>
+    <t>Node0</t>
+  </si>
+  <si>
+    <t>Node1</t>
+  </si>
+  <si>
+    <t>Node4</t>
+  </si>
+  <si>
+    <t>Business process</t>
+  </si>
+  <si>
+    <t>Comment for Node0</t>
+  </si>
+  <si>
+    <t>Information</t>
+  </si>
+  <si>
+    <t>Comment for Node1</t>
+  </si>
+  <si>
+    <t>Node2</t>
+  </si>
+  <si>
+    <t>Immaterial Value</t>
+  </si>
+  <si>
+    <t>Comment for Node2</t>
+  </si>
+  <si>
+    <t>Node3</t>
+  </si>
+  <si>
+    <t>Software</t>
+  </si>
+  <si>
+    <t>Comment for Node3</t>
+  </si>
+  <si>
+    <t>Service</t>
+  </si>
+  <si>
+    <t>Comment for Node4</t>
+  </si>
+  <si>
+    <t>Valid Asset Type</t>
+  </si>
+  <si>
+    <t>Compliance</t>
+  </si>
+  <si>
+    <t>Financial</t>
+  </si>
+  <si>
+    <t>Outsourced service</t>
+  </si>
+  <si>
+    <t>Site</t>
+  </si>
+  <si>
+    <t>Hardware</t>
+  </si>
+  <si>
+    <t>Network</t>
+  </si>
+  <si>
+    <t>Personnel</t>
+  </si>
+  <si>
+    <t>System</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:vt="http://schemas.openxmlformats.org/officeDocument/2006/docPropsVTypes">
-  <numFmts count="1">
-    <numFmt numFmtId="56" formatCode="&quot;上午/下午 &quot;hh&quot;時&quot;mm&quot;分&quot;ss&quot;秒 &quot;"/>
-  </numFmts>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -66,13 +138,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -397,171 +477,198 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
+    </sheetView>
   </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="str">
-        <v>AssetList</v>
-      </c>
-      <c r="B1" t="str">
-        <v>AssetType</v>
-      </c>
-      <c r="C1" t="str">
-        <v>Node0</v>
-      </c>
-      <c r="D1" t="str">
-        <v>Node1</v>
-      </c>
-      <c r="E1" t="str">
-        <v>Node4</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="str">
-        <v>Node1</v>
-      </c>
-      <c r="B2" t="str">
-        <v>Information</v>
-      </c>
-      <c r="C2">
+    <row r="1" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3">
         <v>0.25</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="str">
-        <v>Node2</v>
-      </c>
-      <c r="B3" t="str">
-        <v>Immaterial Value</v>
-      </c>
-      <c r="D3">
+    <row r="4" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4">
         <v>0.95</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" t="str">
-        <v>Node3</v>
-      </c>
-      <c r="B4" t="str">
-        <v>Software</v>
-      </c>
-      <c r="D4">
+    <row r="5" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5">
         <v>1</v>
       </c>
-      <c r="E4">
+      <c r="F5">
         <v>0.75</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" t="str">
-        <v>Node4</v>
-      </c>
-      <c r="B5" t="str">
-        <v>Service</v>
-      </c>
-      <c r="C5">
+    <row r="6" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6">
         <v>1</v>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" t="str">
-        <v>Node0</v>
-      </c>
-      <c r="B6" t="str">
-        <v>Business process</v>
-      </c>
-    </row>
   </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:E6"/>
+    <ignoredError sqref="A1:F6" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:A14"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="str">
-        <v>Valid Asset Type</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="str">
-        <v>Business process</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="str">
-        <v>Compliance</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="str">
-        <v>Financial</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="str">
-        <v>Information</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="str">
-        <v>Immaterial Value</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="str">
-        <v>Outsourced service</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="str">
-        <v>Site</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="str">
-        <v>Software</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="str">
-        <v>Hardware</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="str">
-        <v>Network</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="str">
-        <v>Service</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="str">
-        <v>Personnel</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="str">
-        <v>System</v>
+    <row r="1" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:A14"/>
+    <ignoredError sqref="A1:A14" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>